<commit_message>
Update example outputs with latest data
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/example-vuln-report.xlsx
+++ b/output/example-vuln-report.xlsx
@@ -13,9 +13,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Detail" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'By Package'!$A$1:$H$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'By Package'!$A$1:$H$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'By Host'!$A$1:$I$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Detail'!$A$1:$O$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Detail'!$A$1:$O$103</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -468,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2026-02-17 13:17</t>
+          <t>2026-02-18 16:20</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6">
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10">
@@ -567,7 +567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -667,7 +667,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>elliptic</t>
+          <t>form-data</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -677,12 +677,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6.6.1</t>
+          <t>2.5.4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>GHSA-vjh7-7g9h-fjfh</t>
+          <t>CVE-2025-7783</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pbkdf2</t>
+          <t>elliptic</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -711,12 +711,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.1.3</t>
+          <t>6.6.1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CVE-2025-6545, CVE-2025-6547</t>
+          <t>GHSA-vjh7-7g9h-fjfh</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -735,7 +735,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>form-data</t>
+          <t>pbkdf2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -745,12 +745,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2.5.4</t>
+          <t>3.1.3</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CVE-2025-7783</t>
+          <t>CVE-2025-6545, CVE-2025-6547</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -803,7 +803,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>json-schema</t>
+          <t>growl</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -813,12 +813,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.4.0</t>
+          <t>1.10.0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CVE-2021-3918</t>
+          <t>CVE-2017-16042</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -837,7 +837,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>growl</t>
+          <t>json-schema</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -847,12 +847,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.10.0</t>
+          <t>0.4.0</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CVE-2017-16042</t>
+          <t>CVE-2021-3918</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -871,7 +871,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>cipher-base</t>
+          <t>lodash</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -881,12 +881,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.0.5</t>
+          <t>4.17.12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CVE-2025-9287</t>
+          <t>CVE-2019-10744</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>lodash</t>
+          <t>sha.js</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -915,12 +915,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4.17.12</t>
+          <t>2.4.12</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CVE-2019-10744</t>
+          <t>CVE-2025-9288</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -939,7 +939,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>sha.js</t>
+          <t>cipher-base</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -949,12 +949,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2.4.12</t>
+          <t>1.0.5</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CVE-2025-9288</t>
+          <t>CVE-2025-9287</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1032,7 +1032,7 @@
         <v>9.9</v>
       </c>
       <c r="H13" t="n">
-        <v>11.8</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="14">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>socket.io-parser</t>
+          <t>deep-extend</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1051,12 +1051,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4.2.1</t>
+          <t>0.5.1</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CVE-2022-2421</t>
+          <t>CVE-2018-3750</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>handlebars</t>
+          <t>socket.io-parser</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1085,12 +1085,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4.7.7</t>
+          <t>4.2.1</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>CVE-2021-23369, CVE-2021-23383</t>
+          <t>CVE-2022-2421</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1109,22 +1109,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>fsevents</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>KB5049983</t>
+          <t>1.2.11</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>CVE-2025-21294, CVE-2025-21295, CVE-2025-21296, CVE-2025-21297, CVE-2025-21298, CVE-2025-21307, CVE-2025-21309</t>
+          <t>CVE-2023-45311, GHSA-xv2f-5jw4-v95m</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>handlebars</t>
+          <t>deeply</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1153,12 +1153,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>4.3.0</t>
+          <t>3.1.0</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>CVE-2019-19919</t>
+          <t>CVE-2019-10750</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1177,22 +1177,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>fsevents</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.2.11</t>
+          <t>KB5068787</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CVE-2023-45311, GHSA-xv2f-5jw4-v95m</t>
+          <t>CVE-2025-60724</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1245,22 +1245,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>deeply</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3.1.0</t>
+          <t>KB5063812</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>CVE-2019-10750</t>
+          <t>CVE-2025-50177, CVE-2025-53766</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1279,22 +1279,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>handlebars</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>KB5068840</t>
+          <t>4.7.7</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>CVE-2025-60724</t>
+          <t>CVE-2021-23369, CVE-2021-23383</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>deep-extend</t>
+          <t>cryptiles</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.5.1</t>
+          <t>4.1.2</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>CVE-2018-3750</t>
+          <t>CVE-2018-1000620</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>cryptiles</t>
+          <t>handlebars</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1357,12 +1357,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4.1.2</t>
+          <t>4.3.0</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>CVE-2018-1000620</t>
+          <t>CVE-2019-19919</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1381,32 +1381,32 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>xmlhttprequest-ssl</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>KB5063812</t>
+          <t>1.6.1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CVE-2025-53766</t>
+          <t>CVE-2021-31597</t>
         </is>
       </c>
       <c r="F24" t="n">
         <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>9.800000000000001</v>
+        <v>9.4</v>
       </c>
       <c r="H24" t="n">
-        <v>11.8</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="25">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>pillow</t>
+          <t>cryptography</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1425,22 +1425,22 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12.1.1</t>
+          <t>3.3.2</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>CVE-2021-25289</t>
+          <t>CVE-2020-36242</t>
         </is>
       </c>
       <c r="F25" t="n">
         <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>9.800000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="H25" t="n">
-        <v>11.8</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="26">
@@ -1449,32 +1449,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>xmlhttprequest-ssl</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1.6.1</t>
+          <t>KB5058385</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>CVE-2021-31597</t>
+          <t>CVE-2025-29966, CVE-2025-29967</t>
         </is>
       </c>
       <c r="F26" t="n">
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>9.4</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="H26" t="n">
-        <v>11.4</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="27">
@@ -1483,32 +1483,32 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>cryptography</t>
+          <t>@babel/traverse</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>python</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3.3.2</t>
+          <t>7.23.2</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>CVE-2020-36242</t>
+          <t>CVE-2023-45133</t>
         </is>
       </c>
       <c r="F27" t="n">
         <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>9.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="H27" t="n">
-        <v>11.1</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="28">
@@ -1517,22 +1517,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>@babel/traverse</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>7.23.2</t>
+          <t>KB5065432</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>CVE-2023-45133</t>
+          <t>CVE-2025-53800, CVE-2025-54918</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1561,22 +1561,22 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>KB5058385</t>
+          <t>KB5049983</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>CVE-2025-29833, CVE-2025-29966, CVE-2025-29967</t>
+          <t>CVE-2025-21294, CVE-2025-21295, CVE-2025-21296, CVE-2025-21297, CVE-2025-21298, CVE-2025-21307, CVE-2025-21309</t>
         </is>
       </c>
       <c r="F29" t="n">
         <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>8.800000000000001</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H29" t="n">
-        <v>10.8</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="30">
@@ -1595,22 +1595,22 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>KB5053638</t>
+          <t>KB5055526</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>CVE-2025-24035, CVE-2025-24045, CVE-2025-24064, CVE-2025-26645</t>
+          <t>CVE-2025-26663, CVE-2025-26670, CVE-2025-26686, CVE-2025-27480, CVE-2025-27482, CVE-2025-27491</t>
         </is>
       </c>
       <c r="F30" t="n">
         <v>1</v>
       </c>
       <c r="G30" t="n">
-        <v>8.800000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="H30" t="n">
-        <v>10.8</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="31">
@@ -1629,22 +1629,22 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>KB5062572</t>
+          <t>KB5053603</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>CVE-2024-36350, CVE-2024-36357, CVE-2025-47980, CVE-2025-47981, CVE-2025-48822</t>
+          <t>CVE-2025-24035, CVE-2025-24045, CVE-2025-24064, CVE-2025-24084, CVE-2025-26645</t>
         </is>
       </c>
       <c r="F31" t="n">
         <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>9.800000000000001</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="H31" t="n">
-        <v>10.6</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="32">
@@ -1663,22 +1663,22 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>KB5053603</t>
+          <t>KB5058500</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>CVE-2025-24084</t>
+          <t>CVE-2025-29833, CVE-2025-32710</t>
         </is>
       </c>
       <c r="F32" t="n">
         <v>1</v>
       </c>
       <c r="G32" t="n">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="H32" t="n">
-        <v>10.4</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="33">
@@ -1687,22 +1687,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>xmlhttprequest-ssl</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>KB5055526</t>
+          <t>1.6.2</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>CVE-2025-26663, CVE-2025-26670, CVE-2025-26686, CVE-2025-27480, CVE-2025-27482, CVE-2025-27491</t>
+          <t>CVE-2020-28502</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1731,12 +1731,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>KB5060525</t>
+          <t>KB5052106</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>CVE-2025-29828, CVE-2025-33070, CVE-2025-33071</t>
+          <t>CVE-2025-21376</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1799,19 +1799,19 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>KB5063880</t>
+          <t>KB5060525</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>CVE-2025-50176, CVE-2025-50177, CVE-2025-53778</t>
+          <t>CVE-2025-29828, CVE-2025-33070, CVE-2025-33071</t>
         </is>
       </c>
       <c r="F36" t="n">
         <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>8.800000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="H36" t="n">
         <v>10.1</v>
@@ -1823,32 +1823,32 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>xmlhttprequest-ssl</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.6.2</t>
+          <t>KB5065306</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>CVE-2020-28502</t>
+          <t>CVE-2025-48807, CVE-2025-53799, CVE-2025-55224, CVE-2025-55226, CVE-2025-55228, CVE-2025-55236</t>
         </is>
       </c>
       <c r="F37" t="n">
         <v>1</v>
       </c>
       <c r="G37" t="n">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="H37" t="n">
-        <v>10.1</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="38">
@@ -1867,22 +1867,22 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>KB5052106</t>
+          <t>KB5063880</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>CVE-2025-21376</t>
+          <t>CVE-2025-50176, CVE-2025-53778</t>
         </is>
       </c>
       <c r="F38" t="n">
         <v>1</v>
       </c>
       <c r="G38" t="n">
-        <v>8.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="H38" t="n">
-        <v>10.1</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="39">
@@ -1901,22 +1901,22 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>KB5058500</t>
+          <t>KB5073457</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>CVE-2025-32710</t>
+          <t>CVE-2026-20822</t>
         </is>
       </c>
       <c r="F39" t="n">
         <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="H39" t="n">
-        <v>10.1</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="40">
@@ -1935,22 +1935,22 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>KB5065306</t>
+          <t>KB5068840</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>CVE-2025-48807, CVE-2025-53799, CVE-2025-55224, CVE-2025-55226</t>
+          <t>CVE-2025-60716</t>
         </is>
       </c>
       <c r="F40" t="n">
         <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>7.8</v>
+        <v>7</v>
       </c>
       <c r="H40" t="n">
-        <v>9.800000000000001</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41">
@@ -1969,94 +1969,26 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>KB5065432</t>
+          <t>KB5062572</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>CVE-2025-53800, CVE-2025-54918, CVE-2025-55228, CVE-2025-55236</t>
+          <t>CVE-2024-36350, CVE-2024-36357, CVE-2025-47980, CVE-2025-47981, CVE-2025-48822</t>
         </is>
       </c>
       <c r="F41" t="n">
         <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>8.800000000000001</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H41" t="n">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Microsoft Windows Server 2022</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>win:s2022</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>KB5073457</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>CVE-2026-20822</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" t="n">
-        <v>7.8</v>
-      </c>
-      <c r="H42" t="n">
-        <v>9.800000000000001</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Microsoft Windows Server 2022</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>win:s2022</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>KB5068787</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>CVE-2025-60716</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" t="n">
-        <v>7</v>
-      </c>
-      <c r="H43" t="n">
-        <v>9</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H43"/>
+  <autoFilter ref="A1:H41"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2139,12 +2071,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2158,10 +2090,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="n">
         <v>8</v>
@@ -2176,12 +2108,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2195,10 +2127,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3" t="n">
         <v>8</v>
@@ -2293,7 +2225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O104"/>
+  <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2401,7 +2333,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GHSA-vjh7-7g9h-fjfh</t>
+          <t>CVE-2025-7783</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2414,7 +2346,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>elliptic</t>
+          <t>form-data</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2424,12 +2356,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>6.4.0</t>
+          <t>2.3.1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>6.6.1</t>
+          <t>2.5.4</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -2464,7 +2396,7 @@
       </c>
       <c r="O2" s="2" t="inlineStr">
         <is>
-          <t>https://github.com/advisories/GHSA-vjh7-7g9h-fjfh</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
         </is>
       </c>
     </row>
@@ -2474,7 +2406,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CVE-2025-6545</t>
+          <t>CVE-2025-7783</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2487,7 +2419,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>pbkdf2</t>
+          <t>form-data</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2497,12 +2429,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3.0.12</t>
+          <t>2.1.4</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>3.1.3</t>
+          <t>2.5.4</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -2537,7 +2469,7 @@
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
         </is>
       </c>
     </row>
@@ -2547,7 +2479,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CVE-2025-6547</t>
+          <t>CVE-2025-7783</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2560,7 +2492,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>pbkdf2</t>
+          <t>form-data</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2570,12 +2502,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3.0.12</t>
+          <t>4.0.1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>3.1.3</t>
+          <t>4.0.4</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -2610,7 +2542,7 @@
       </c>
       <c r="O4" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
         </is>
       </c>
     </row>
@@ -2620,7 +2552,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CVE-2025-6547</t>
+          <t>CVE-2025-7783</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2633,7 +2565,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>pbkdf2</t>
+          <t>form-data</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2643,12 +2575,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3.0.14</t>
+          <t>2.1.4</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3.1.3</t>
+          <t>2.5.4</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -2683,7 +2615,7 @@
       </c>
       <c r="O5" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
         </is>
       </c>
     </row>
@@ -2693,7 +2625,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CVE-2025-6545</t>
+          <t>GHSA-vjh7-7g9h-fjfh</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2706,7 +2638,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>pbkdf2</t>
+          <t>elliptic</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2716,12 +2648,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3.1.2</t>
+          <t>6.5.2</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>3.1.3</t>
+          <t>6.6.1</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -2756,7 +2688,7 @@
       </c>
       <c r="O6" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
+          <t>https://github.com/advisories/GHSA-vjh7-7g9h-fjfh</t>
         </is>
       </c>
     </row>
@@ -2766,7 +2698,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CVE-2025-7783</t>
+          <t>GHSA-vjh7-7g9h-fjfh</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2779,7 +2711,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>form-data</t>
+          <t>elliptic</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2789,22 +2721,22 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4.0.1</t>
+          <t>6.4.0</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>4.0.4</t>
+          <t>6.6.1</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -2829,7 +2761,7 @@
       </c>
       <c r="O7" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
+          <t>https://github.com/advisories/GHSA-vjh7-7g9h-fjfh</t>
         </is>
       </c>
     </row>
@@ -2912,7 +2844,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CVE-2025-7783</t>
+          <t>CVE-2025-6547</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2925,7 +2857,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>form-data</t>
+          <t>pbkdf2</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2935,22 +2867,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2.3.1</t>
+          <t>3.1.2</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2.5.4</t>
+          <t>3.1.3</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -2975,7 +2907,7 @@
       </c>
       <c r="O9" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
         </is>
       </c>
     </row>
@@ -2985,7 +2917,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CVE-2025-6545</t>
+          <t>CVE-2025-6547</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3008,7 +2940,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3.0.14</t>
+          <t>3.0.12</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -3018,12 +2950,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -3048,7 +2980,7 @@
       </c>
       <c r="O10" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
         </is>
       </c>
     </row>
@@ -3058,7 +2990,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CVE-2025-7783</t>
+          <t>CVE-2025-6547</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -3071,7 +3003,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>form-data</t>
+          <t>pbkdf2</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -3081,12 +3013,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2.1.4</t>
+          <t>3.0.17</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2.5.4</t>
+          <t>3.1.3</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -3121,7 +3053,7 @@
       </c>
       <c r="O11" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
         </is>
       </c>
     </row>
@@ -3131,7 +3063,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CVE-2025-6545</t>
+          <t>CVE-2025-6547</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -3154,7 +3086,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>3.0.17</t>
+          <t>3.0.14</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -3164,12 +3096,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -3194,7 +3126,7 @@
       </c>
       <c r="O12" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
         </is>
       </c>
     </row>
@@ -3204,7 +3136,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CVE-2025-7783</t>
+          <t>CVE-2025-6545</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -3217,7 +3149,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>form-data</t>
+          <t>pbkdf2</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -3227,22 +3159,22 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2.1.4</t>
+          <t>3.0.17</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2.5.4</t>
+          <t>3.1.3</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -3267,7 +3199,7 @@
       </c>
       <c r="O13" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3209,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GHSA-vjh7-7g9h-fjfh</t>
+          <t>CVE-2025-6545</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3290,7 +3222,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>elliptic</t>
+          <t>pbkdf2</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -3300,12 +3232,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>6.5.2</t>
+          <t>3.0.12</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>6.6.1</t>
+          <t>3.1.3</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -3340,7 +3272,7 @@
       </c>
       <c r="O14" s="2" t="inlineStr">
         <is>
-          <t>https://github.com/advisories/GHSA-vjh7-7g9h-fjfh</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
         </is>
       </c>
     </row>
@@ -3350,7 +3282,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CVE-2025-6547</t>
+          <t>CVE-2025-6545</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3373,7 +3305,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3.0.17</t>
+          <t>3.0.14</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -3383,12 +3315,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -3413,7 +3345,7 @@
       </c>
       <c r="O15" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
         </is>
       </c>
     </row>
@@ -3423,7 +3355,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CVE-2025-6547</t>
+          <t>CVE-2025-6545</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3486,7 +3418,7 @@
       </c>
       <c r="O16" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
         </is>
       </c>
     </row>
@@ -3569,7 +3501,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CVE-2021-44906</t>
+          <t>CVE-2018-3750</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -3582,7 +3514,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>minimist</t>
+          <t>deep-extend</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -3592,12 +3524,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>1.2.0</t>
+          <t>0.4.2</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1.2.6</t>
+          <t>0.5.1</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -3632,7 +3564,7 @@
       </c>
       <c r="O18" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2018-3750</t>
         </is>
       </c>
     </row>
@@ -3642,7 +3574,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CVE-2016-9535</t>
+          <t>CVE-2022-2421</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3655,32 +3587,32 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>socket.io-parser</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>KB5048654</t>
+          <t>2.3.1</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>KB5066782</t>
+          <t>4.2.1</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>i-0c8104214f010bf57</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -3705,7 +3637,7 @@
       </c>
       <c r="O19" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2016-9535</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2022-2421</t>
         </is>
       </c>
     </row>
@@ -3715,7 +3647,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CVE-2021-44906</t>
+          <t>CVE-2023-45311</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -3728,7 +3660,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>minimist</t>
+          <t>fsevents</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -3738,22 +3670,22 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0.0.8</t>
+          <t>1.1.1</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0.2.4</t>
+          <t>1.2.11</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -3778,7 +3710,7 @@
       </c>
       <c r="O20" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2023-45311</t>
         </is>
       </c>
     </row>
@@ -3788,7 +3720,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CVE-2022-2421</t>
+          <t>CVE-2023-45311</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -3801,7 +3733,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>socket.io-parser</t>
+          <t>fsevents</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -3811,12 +3743,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2.3.1</t>
+          <t>1.2.9</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>4.2.1</t>
+          <t>1.2.11</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -3851,7 +3783,7 @@
       </c>
       <c r="O21" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2022-2421</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2023-45311</t>
         </is>
       </c>
     </row>
@@ -3861,7 +3793,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CVE-2021-23383</t>
+          <t>CVE-2019-10750</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -3874,7 +3806,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>handlebars</t>
+          <t>deeply</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -3884,12 +3816,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>4.0.11</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>4.7.7</t>
+          <t>3.1.0</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -3924,7 +3856,7 @@
       </c>
       <c r="O22" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-23383</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10750</t>
         </is>
       </c>
     </row>
@@ -3934,7 +3866,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CVE-2025-21298</t>
+          <t>CVE-2025-60724</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -3962,7 +3894,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>KB5049983</t>
+          <t>KB5068787</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -3997,7 +3929,7 @@
       </c>
       <c r="O23" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21298</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-60724</t>
         </is>
       </c>
     </row>
@@ -4030,12 +3962,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1.2.0</t>
+          <t>0.0.10</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1.2.6</t>
+          <t>0.2.4</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -4080,7 +4012,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CVE-2025-47981</t>
+          <t>CVE-2021-44906</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -4093,32 +4025,32 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>minimist</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>KB5048654</t>
+          <t>1.2.0</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>KB5062572</t>
+          <t>1.2.6</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>i-0c8104214f010bf57</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -4143,7 +4075,7 @@
       </c>
       <c r="O25" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-47981</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
       </c>
     </row>
@@ -4153,7 +4085,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CVE-2019-19919</t>
+          <t>CVE-2021-44906</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -4166,7 +4098,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>handlebars</t>
+          <t>minimist</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -4176,12 +4108,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>4.0.11</t>
+          <t>0.0.8</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>4.3.0</t>
+          <t>0.2.4</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -4216,7 +4148,7 @@
       </c>
       <c r="O26" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-19919</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
       </c>
     </row>
@@ -4226,7 +4158,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CVE-2023-45311</t>
+          <t>CVE-2021-44906</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -4239,7 +4171,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>fsevents</t>
+          <t>minimist</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -4249,22 +4181,22 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1.1.1</t>
+          <t>1.2.5</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1.2.11</t>
+          <t>1.2.6</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-1-165.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-017ae4a71a0aeb374</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -4289,7 +4221,7 @@
       </c>
       <c r="O27" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2023-45311</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
       </c>
     </row>
@@ -4299,7 +4231,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>CVE-2025-59287</t>
+          <t>CVE-2021-44906</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -4312,32 +4244,32 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>minimist</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>KB5048654</t>
+          <t>1.2.5</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>KB5070884</t>
+          <t>1.2.6</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>i-0c8104214f010bf57</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -4362,7 +4294,7 @@
       </c>
       <c r="O28" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-59287</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
       </c>
     </row>
@@ -4372,7 +4304,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CVE-2019-10750</t>
+          <t>CVE-2021-44906</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -4385,7 +4317,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>deeply</t>
+          <t>minimist</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -4395,22 +4327,22 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>1.0.0</t>
+          <t>0.0.8</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>3.1.0</t>
+          <t>0.2.4</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -4435,7 +4367,7 @@
       </c>
       <c r="O29" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10750</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
       </c>
     </row>
@@ -4445,7 +4377,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CVE-2025-21307</t>
+          <t>CVE-2021-44906</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -4458,32 +4390,32 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>minimist</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>KB5048654</t>
+          <t>1.2.5</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>KB5049983</t>
+          <t>1.2.6</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>i-0c8104214f010bf57</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -4508,7 +4440,7 @@
       </c>
       <c r="O30" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21307</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
       </c>
     </row>
@@ -4518,7 +4450,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>CVE-2021-3918</t>
+          <t>CVE-2021-44906</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -4531,7 +4463,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>json-schema</t>
+          <t>minimist</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -4541,12 +4473,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>0.2.3</t>
+          <t>1.2.0</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>0.4.0</t>
+          <t>1.2.6</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -4581,7 +4513,7 @@
       </c>
       <c r="O31" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-3918</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
       </c>
     </row>
@@ -4591,7 +4523,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CVE-2025-60724</t>
+          <t>CVE-2025-47981</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -4619,7 +4551,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>KB5068840</t>
+          <t>KB5062572</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -4654,7 +4586,7 @@
       </c>
       <c r="O32" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-60724</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-47981</t>
         </is>
       </c>
     </row>
@@ -4664,7 +4596,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>CVE-2021-44906</t>
+          <t>CVE-2025-59287</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -4677,32 +4609,32 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>minimist</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0.0.8</t>
+          <t>KB5048654</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>0.2.4</t>
+          <t>KB5070884</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0c8104214f010bf57</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -4727,7 +4659,7 @@
       </c>
       <c r="O33" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-59287</t>
         </is>
       </c>
     </row>
@@ -4737,7 +4669,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CVE-2021-44906</t>
+          <t>CVE-2025-53766</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -4750,32 +4682,32 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>minimist</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>1.2.5</t>
+          <t>KB5048654</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>1.2.6</t>
+          <t>KB5063812</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0c8104214f010bf57</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -4800,7 +4732,7 @@
       </c>
       <c r="O34" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53766</t>
         </is>
       </c>
     </row>
@@ -4810,7 +4742,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CVE-2021-23369</t>
+          <t>CVE-2021-23383</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -4873,7 +4805,7 @@
       </c>
       <c r="O35" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-23369</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-23383</t>
         </is>
       </c>
     </row>
@@ -4883,7 +4815,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CVE-2021-3918</t>
+          <t>CVE-2018-1000620</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -4896,7 +4828,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>json-schema</t>
+          <t>cryptiles</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4906,12 +4838,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0.2.3</t>
+          <t>3.1.2</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>0.4.0</t>
+          <t>4.1.2</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -4946,7 +4878,7 @@
       </c>
       <c r="O36" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-3918</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2018-1000620</t>
         </is>
       </c>
     </row>
@@ -4956,7 +4888,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CVE-2017-16042</t>
+          <t>CVE-2019-19919</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -4969,7 +4901,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>growl</t>
+          <t>handlebars</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4979,22 +4911,22 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>1.9.2</t>
+          <t>4.0.11</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1.10.0</t>
+          <t>4.3.0</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -5019,7 +4951,7 @@
       </c>
       <c r="O37" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2017-16042</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-19919</t>
         </is>
       </c>
     </row>
@@ -5029,7 +4961,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CVE-2017-16042</t>
+          <t>CVE-2016-9535</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -5042,32 +4974,32 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>growl</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>1.9.2</t>
+          <t>KB5048654</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1.10.0</t>
+          <t>KB5066782</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0c8104214f010bf57</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -5092,7 +5024,7 @@
       </c>
       <c r="O38" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2017-16042</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2016-9535</t>
         </is>
       </c>
     </row>
@@ -5102,7 +5034,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CVE-2018-3750</t>
+          <t>CVE-2017-16042</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -5115,7 +5047,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>deep-extend</t>
+          <t>growl</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -5125,12 +5057,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>0.4.2</t>
+          <t>1.9.2</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>0.5.1</t>
+          <t>1.10.0</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -5165,7 +5097,7 @@
       </c>
       <c r="O39" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2018-3750</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2017-16042</t>
         </is>
       </c>
     </row>
@@ -5175,7 +5107,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CVE-2018-1000620</t>
+          <t>CVE-2017-16042</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -5188,7 +5120,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>cryptiles</t>
+          <t>growl</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -5198,12 +5130,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>3.1.2</t>
+          <t>1.9.2</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>4.1.2</t>
+          <t>1.10.0</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -5238,7 +5170,7 @@
       </c>
       <c r="O40" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2018-1000620</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2017-16042</t>
         </is>
       </c>
     </row>
@@ -5248,7 +5180,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>CVE-2021-44906</t>
+          <t>CVE-2021-3918</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -5261,7 +5193,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>minimist</t>
+          <t>json-schema</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5271,22 +5203,22 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>1.2.5</t>
+          <t>0.2.3</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>1.2.6</t>
+          <t>0.4.0</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>ip-172-17-1-165.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>i-017ae4a71a0aeb374</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -5311,7 +5243,7 @@
       </c>
       <c r="O41" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-3918</t>
         </is>
       </c>
     </row>
@@ -5321,7 +5253,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>CVE-2021-44906</t>
+          <t>CVE-2021-3918</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -5334,7 +5266,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>minimist</t>
+          <t>json-schema</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5344,12 +5276,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>1.2.5</t>
+          <t>0.2.3</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1.2.6</t>
+          <t>0.4.0</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -5384,7 +5316,7 @@
       </c>
       <c r="O42" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-3918</t>
         </is>
       </c>
     </row>
@@ -5394,7 +5326,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>CVE-2021-44906</t>
+          <t>CVE-2021-23369</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -5407,7 +5339,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>minimist</t>
+          <t>handlebars</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5417,12 +5349,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>0.0.10</t>
+          <t>4.0.11</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>0.2.4</t>
+          <t>4.7.7</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -5457,7 +5389,7 @@
       </c>
       <c r="O43" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-23369</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5399,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CVE-2025-53766</t>
+          <t>CVE-2025-21307</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -5495,7 +5427,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>KB5063812</t>
+          <t>KB5049983</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -5530,7 +5462,7 @@
       </c>
       <c r="O44" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53766</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21307</t>
         </is>
       </c>
     </row>
@@ -5540,7 +5472,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CVE-2023-45311</t>
+          <t>CVE-2025-21298</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -5553,32 +5485,32 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>fsevents</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>1.2.9</t>
+          <t>KB5048654</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1.2.11</t>
+          <t>KB5049983</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0c8104214f010bf57</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -5603,17 +5535,17 @@
       </c>
       <c r="O45" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2023-45311</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21298</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>11.8</v>
+        <v>11.4</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>CVE-2021-25289</t>
+          <t>CVE-2021-31597</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -5622,26 +5554,26 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>9.800000000000001</v>
+        <v>9.4</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>pillow</t>
+          <t>xmlhttprequest-ssl</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>python</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>10.4.0</t>
+          <t>1.5.3</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>12.1.1</t>
+          <t>1.6.1</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -5676,17 +5608,17 @@
       </c>
       <c r="O46" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-25289</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-31597</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>11.4</v>
+        <v>11.1</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>CVE-2021-31597</t>
+          <t>CVE-2019-10744</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -5695,11 +5627,11 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>9.4</v>
+        <v>9.1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>xmlhttprequest-ssl</t>
+          <t>lodash</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5709,12 +5641,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>1.5.3</t>
+          <t>4.17.4</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>1.6.1</t>
+          <t>4.17.12</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -5749,7 +5681,7 @@
       </c>
       <c r="O47" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-31597</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
         </is>
       </c>
     </row>
@@ -5759,7 +5691,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>CVE-2025-9287</t>
+          <t>CVE-2019-10744</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -5772,7 +5704,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>cipher-base</t>
+          <t>lodash</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5782,12 +5714,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>1.0.3</t>
+          <t>3.10.1</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1.0.5</t>
+          <t>4.17.12</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -5822,7 +5754,7 @@
       </c>
       <c r="O48" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
         </is>
       </c>
     </row>
@@ -5832,7 +5764,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>CVE-2025-9287</t>
+          <t>CVE-2019-10744</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -5845,7 +5777,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>cipher-base</t>
+          <t>lodash</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5855,12 +5787,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>1.0.4</t>
+          <t>4.17.5</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>1.0.5</t>
+          <t>4.17.12</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -5895,7 +5827,7 @@
       </c>
       <c r="O49" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
         </is>
       </c>
     </row>
@@ -5905,7 +5837,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>CVE-2020-36242</t>
+          <t>CVE-2019-10744</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -5918,22 +5850,22 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>cryptography</t>
+          <t>lodash</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>python</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>3.2.1</t>
+          <t>4.17.4</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>3.3.2</t>
+          <t>4.17.12</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -5968,7 +5900,7 @@
       </c>
       <c r="O50" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2020-36242</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
         </is>
       </c>
     </row>
@@ -5978,7 +5910,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>CVE-2019-10744</t>
+          <t>CVE-2020-36242</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -5991,22 +5923,22 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>lodash</t>
+          <t>cryptography</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>python</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>4.17.4</t>
+          <t>3.2.1</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>4.17.12</t>
+          <t>3.3.2</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -6041,7 +5973,7 @@
       </c>
       <c r="O51" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2020-36242</t>
         </is>
       </c>
     </row>
@@ -6074,7 +6006,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2.4.11</t>
+          <t>2.4.10</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -6084,12 +6016,12 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -6124,7 +6056,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>CVE-2019-10744</t>
+          <t>CVE-2025-9288</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -6137,7 +6069,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>lodash</t>
+          <t>sha.js</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6147,12 +6079,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>4.17.4</t>
+          <t>2.4.11</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>4.17.12</t>
+          <t>2.4.12</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -6187,7 +6119,7 @@
       </c>
       <c r="O53" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9288</t>
         </is>
       </c>
     </row>
@@ -6197,7 +6129,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>CVE-2019-10744</t>
+          <t>CVE-2025-9288</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -6210,7 +6142,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>lodash</t>
+          <t>sha.js</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6220,22 +6152,22 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>4.17.5</t>
+          <t>2.4.8</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>4.17.12</t>
+          <t>2.4.12</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -6260,7 +6192,7 @@
       </c>
       <c r="O54" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9288</t>
         </is>
       </c>
     </row>
@@ -6270,7 +6202,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>CVE-2019-10744</t>
+          <t>CVE-2025-9287</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -6283,7 +6215,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>lodash</t>
+          <t>cipher-base</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6293,12 +6225,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>3.10.1</t>
+          <t>1.0.3</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>4.17.12</t>
+          <t>1.0.5</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -6333,7 +6265,7 @@
       </c>
       <c r="O55" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
         </is>
       </c>
     </row>
@@ -6343,7 +6275,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>CVE-2025-9288</t>
+          <t>CVE-2025-9287</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -6356,7 +6288,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>sha.js</t>
+          <t>cipher-base</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6366,12 +6298,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2.4.10</t>
+          <t>1.0.4</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2.4.12</t>
+          <t>1.0.5</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -6406,7 +6338,7 @@
       </c>
       <c r="O56" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9288</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
         </is>
       </c>
     </row>
@@ -6416,7 +6348,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>CVE-2025-9288</t>
+          <t>CVE-2025-9287</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -6429,7 +6361,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>sha.js</t>
+          <t>cipher-base</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6439,12 +6371,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2.4.8</t>
+          <t>1.0.4</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2.4.12</t>
+          <t>1.0.5</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -6479,17 +6411,17 @@
       </c>
       <c r="O57" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9288</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>11.1</v>
+        <v>10.8</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>CVE-2025-9287</t>
+          <t>CVE-2025-29966</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -6498,36 +6430,36 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>9.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>cipher-base</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>1.0.4</t>
+          <t>KB5048654</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>1.0.5</t>
+          <t>KB5058385</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0c8104214f010bf57</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -6552,7 +6484,7 @@
       </c>
       <c r="O58" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29966</t>
         </is>
       </c>
     </row>
@@ -6635,7 +6567,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>CVE-2025-29966</t>
+          <t>CVE-2025-54918</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -6663,7 +6595,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>KB5058385</t>
+          <t>KB5065432</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -6698,7 +6630,7 @@
       </c>
       <c r="O60" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29966</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-54918</t>
         </is>
       </c>
     </row>
@@ -6736,7 +6668,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>KB5053638</t>
+          <t>KB5053603</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -6854,7 +6786,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>CVE-2025-54918</t>
+          <t>CVE-2025-29967</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -6882,7 +6814,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>KB5065432</t>
+          <t>KB5058385</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -6917,17 +6849,17 @@
       </c>
       <c r="O63" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-54918</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29967</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>10.8</v>
+        <v>10.6</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>CVE-2025-29967</t>
+          <t>CVE-2025-48822</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -6936,7 +6868,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>8.800000000000001</v>
+        <v>8.6</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -6955,7 +6887,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>KB5058385</t>
+          <t>KB5062572</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -6990,17 +6922,17 @@
       </c>
       <c r="O64" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29967</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-48822</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>10.6</v>
+        <v>10.4</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>CVE-2025-48822</t>
+          <t>CVE-2025-24084</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -7009,7 +6941,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>8.6</v>
+        <v>8.4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -7028,7 +6960,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>KB5062572</t>
+          <t>KB5053603</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -7063,17 +6995,17 @@
       </c>
       <c r="O65" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-48822</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24084</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>10.4</v>
+        <v>10.1</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>CVE-2025-24084</t>
+          <t>CVE-2025-21295</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -7082,7 +7014,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -7101,7 +7033,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>KB5053603</t>
+          <t>KB5049983</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -7136,7 +7068,7 @@
       </c>
       <c r="O66" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24084</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21295</t>
         </is>
       </c>
     </row>
@@ -7219,7 +7151,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>CVE-2025-33071</t>
+          <t>CVE-2025-24035</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -7247,7 +7179,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>KB5060525</t>
+          <t>KB5053603</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -7282,7 +7214,7 @@
       </c>
       <c r="O68" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-33071</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24035</t>
         </is>
       </c>
     </row>
@@ -7292,7 +7224,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>CVE-2025-49735</t>
+          <t>CVE-2025-21309</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -7320,7 +7252,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>KB5060526</t>
+          <t>KB5049983</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -7355,7 +7287,7 @@
       </c>
       <c r="O69" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-49735</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21309</t>
         </is>
       </c>
     </row>
@@ -7365,7 +7297,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>CVE-2025-50177</t>
+          <t>CVE-2025-32710</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -7393,7 +7325,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>KB5063880</t>
+          <t>KB5058500</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -7428,7 +7360,7 @@
       </c>
       <c r="O70" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-50177</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-32710</t>
         </is>
       </c>
     </row>
@@ -7438,7 +7370,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>CVE-2025-29828</t>
+          <t>CVE-2025-27480</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -7466,7 +7398,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>KB5060525</t>
+          <t>KB5055526</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -7501,7 +7433,7 @@
       </c>
       <c r="O71" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29828</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27480</t>
         </is>
       </c>
     </row>
@@ -7584,7 +7516,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>CVE-2025-24045</t>
+          <t>CVE-2020-28502</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -7597,32 +7529,32 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>xmlhttprequest-ssl</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>KB5048654</t>
+          <t>1.5.3</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>KB5053638</t>
+          <t>1.6.2</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>i-0c8104214f010bf57</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -7647,7 +7579,7 @@
       </c>
       <c r="O73" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24045</t>
+          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2020-28502</t>
         </is>
       </c>
     </row>
@@ -7657,7 +7589,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>CVE-2020-28502</t>
+          <t>CVE-2025-21376</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -7670,32 +7602,32 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>xmlhttprequest-ssl</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>1.5.3</t>
+          <t>KB5048654</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>1.6.2</t>
+          <t>KB5052106</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0c8104214f010bf57</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -7720,7 +7652,7 @@
       </c>
       <c r="O74" s="2" t="inlineStr">
         <is>
-          <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2020-28502</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21376</t>
         </is>
       </c>
     </row>
@@ -7730,7 +7662,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>CVE-2025-21376</t>
+          <t>CVE-2025-49735</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -7758,7 +7690,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>KB5052106</t>
+          <t>KB5060526</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -7793,7 +7725,7 @@
       </c>
       <c r="O75" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21376</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-49735</t>
         </is>
       </c>
     </row>
@@ -7803,7 +7735,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>CVE-2025-32710</t>
+          <t>CVE-2025-50177</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -7831,7 +7763,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>KB5058500</t>
+          <t>KB5063812</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -7866,7 +7798,7 @@
       </c>
       <c r="O76" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-32710</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-50177</t>
         </is>
       </c>
     </row>
@@ -7876,7 +7808,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>CVE-2025-27480</t>
+          <t>CVE-2025-29828</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -7904,7 +7836,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>KB5055526</t>
+          <t>KB5060525</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -7939,7 +7871,7 @@
       </c>
       <c r="O77" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27480</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29828</t>
         </is>
       </c>
     </row>
@@ -7949,7 +7881,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>CVE-2025-24064</t>
+          <t>CVE-2025-33071</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -7977,7 +7909,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>KB5053638</t>
+          <t>KB5060525</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -8012,7 +7944,7 @@
       </c>
       <c r="O78" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24064</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-33071</t>
         </is>
       </c>
     </row>
@@ -8022,7 +7954,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>CVE-2025-21309</t>
+          <t>CVE-2025-21297</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -8085,7 +8017,7 @@
       </c>
       <c r="O79" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21309</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21297</t>
         </is>
       </c>
     </row>
@@ -8168,7 +8100,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>CVE-2025-24035</t>
+          <t>CVE-2025-26670</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -8196,7 +8128,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>KB5053638</t>
+          <t>KB5055526</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -8231,7 +8163,7 @@
       </c>
       <c r="O81" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24035</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-26670</t>
         </is>
       </c>
     </row>
@@ -8241,7 +8173,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>CVE-2025-21297</t>
+          <t>CVE-2025-24045</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -8269,7 +8201,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>KB5049983</t>
+          <t>KB5053603</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
@@ -8304,7 +8236,7 @@
       </c>
       <c r="O82" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21297</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24045</t>
         </is>
       </c>
     </row>
@@ -8314,7 +8246,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>CVE-2025-21295</t>
+          <t>CVE-2025-27482</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -8342,7 +8274,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>KB5049983</t>
+          <t>KB5055526</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -8377,7 +8309,7 @@
       </c>
       <c r="O83" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21295</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27482</t>
         </is>
       </c>
     </row>
@@ -8387,7 +8319,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>CVE-2025-26670</t>
+          <t>CVE-2025-24064</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -8415,7 +8347,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>KB5055526</t>
+          <t>KB5053603</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -8450,17 +8382,17 @@
       </c>
       <c r="O84" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-26670</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24064</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>10.1</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>CVE-2025-27482</t>
+          <t>CVE-2025-55228</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -8469,7 +8401,7 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -8488,7 +8420,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>KB5055526</t>
+          <t>KB5065306</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -8523,7 +8455,7 @@
       </c>
       <c r="O85" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27482</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55228</t>
         </is>
       </c>
     </row>
@@ -8533,7 +8465,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>CVE-2025-55224</t>
+          <t>CVE-2025-50176</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -8561,7 +8493,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>KB5065306</t>
+          <t>KB5063880</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -8596,7 +8528,7 @@
       </c>
       <c r="O86" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55224</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-50176</t>
         </is>
       </c>
     </row>
@@ -8606,7 +8538,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>CVE-2025-55228</t>
+          <t>CVE-2025-53800</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -8669,7 +8601,7 @@
       </c>
       <c r="O87" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55228</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53800</t>
         </is>
       </c>
     </row>
@@ -8752,7 +8684,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>CVE-2025-53800</t>
+          <t>CVE-2025-55224</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -8780,7 +8712,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>KB5065432</t>
+          <t>KB5065306</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -8815,17 +8747,17 @@
       </c>
       <c r="O89" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53800</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55224</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>9.800000000000001</v>
+        <v>9.76</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>CVE-2025-50176</t>
+          <t>GHSA-xv2f-5jw4-v95m</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -8834,36 +8766,36 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>7.8</v>
+        <v>7.76</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Microsoft Windows Server 2022</t>
+          <t>fsevents</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>win:s2022</t>
+          <t>npm</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>KB5048654</t>
+          <t>1.2.9</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>KB5063880</t>
+          <t>1.2.11</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>i-0c8104214f010bf57</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -8888,7 +8820,7 @@
       </c>
       <c r="O90" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-50176</t>
+          <t>https://github.com/advisories/GHSA-xv2f-5jw4-v95m</t>
         </is>
       </c>
     </row>
@@ -8967,11 +8899,11 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>9.76</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>GHSA-xv2f-5jw4-v95m</t>
+          <t>CVE-2025-29833</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -8980,36 +8912,36 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>7.76</v>
+        <v>7.7</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>fsevents</t>
+          <t>Microsoft Windows Server 2022</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>npm</t>
+          <t>win:s2022</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>1.2.9</t>
+          <t>KB5048654</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>1.2.11</t>
+          <t>KB5058500</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0c8104214f010bf57</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -9034,17 +8966,17 @@
       </c>
       <c r="O92" s="2" t="inlineStr">
         <is>
-          <t>https://github.com/advisories/GHSA-xv2f-5jw4-v95m</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29833</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>9.699999999999999</v>
+        <v>9.5</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>CVE-2025-29833</t>
+          <t>CVE-2025-26686</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -9053,7 +8985,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>7.7</v>
+        <v>7.5</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -9072,7 +9004,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>KB5058385</t>
+          <t>KB5055526</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -9107,7 +9039,7 @@
       </c>
       <c r="O93" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29833</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-26686</t>
         </is>
       </c>
     </row>
@@ -9117,7 +9049,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>CVE-2025-26686</t>
+          <t>CVE-2025-21296</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -9145,7 +9077,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>KB5055526</t>
+          <t>KB5049983</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -9180,17 +9112,17 @@
       </c>
       <c r="O94" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-26686</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21296</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>9.5</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>CVE-2025-21296</t>
+          <t>CVE-2025-55236</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -9199,7 +9131,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -9218,7 +9150,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>KB5049983</t>
+          <t>KB5065306</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -9253,17 +9185,17 @@
       </c>
       <c r="O95" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21296</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55236</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>9.300000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>CVE-2025-55236</t>
+          <t>CVE-2025-27491</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -9272,7 +9204,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>7.3</v>
+        <v>7.1</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -9291,7 +9223,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>KB5065432</t>
+          <t>KB5055526</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -9326,17 +9258,17 @@
       </c>
       <c r="O96" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55236</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27491</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>CVE-2025-27491</t>
+          <t>CVE-2025-60716</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -9345,7 +9277,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>7.1</v>
+        <v>7</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -9364,7 +9296,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>KB5055526</t>
+          <t>KB5068840</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -9399,17 +9331,17 @@
       </c>
       <c r="O97" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27491</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-60716</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>9</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>CVE-2025-60716</t>
+          <t>CVE-2025-48807</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -9418,7 +9350,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -9437,7 +9369,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>KB5068787</t>
+          <t>KB5065306</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
@@ -9472,7 +9404,7 @@
       </c>
       <c r="O98" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-60716</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-48807</t>
         </is>
       </c>
     </row>
@@ -9482,7 +9414,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>CVE-2025-48807</t>
+          <t>CVE-2025-55226</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -9545,17 +9477,17 @@
       </c>
       <c r="O99" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-48807</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55226</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>8.699999999999999</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>CVE-2025-55226</t>
+          <t>CVE-2025-47980</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -9564,7 +9496,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -9583,7 +9515,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>KB5065306</t>
+          <t>KB5062572</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -9618,17 +9550,17 @@
       </c>
       <c r="O100" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55226</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-47980</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>8.199999999999999</v>
+        <v>7.6</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>CVE-2025-47980</t>
+          <t>CVE-2024-36357</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -9637,7 +9569,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>6.2</v>
+        <v>5.6</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -9691,7 +9623,7 @@
       </c>
       <c r="O101" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-47980</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2024-36357</t>
         </is>
       </c>
     </row>
@@ -9701,7 +9633,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>CVE-2024-36357</t>
+          <t>CVE-2024-36350</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -9764,17 +9696,17 @@
       </c>
       <c r="O102" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2024-36357</t>
+          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2024-36350</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>7.6</v>
+        <v>7.5</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>CVE-2024-36350</t>
+          <t>CVE-2025-53799</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -9783,7 +9715,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -9802,7 +9734,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>KB5062572</t>
+          <t>KB5065306</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -9837,85 +9769,12 @@
       </c>
       <c r="O103" s="2" t="inlineStr">
         <is>
-          <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2024-36350</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>CVE-2025-53799</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Critical</t>
-        </is>
-      </c>
-      <c r="D104" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>Microsoft Windows Server 2022</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>win:s2022</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>KB5048654</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>KB5065306</t>
-        </is>
-      </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>ip-172-17-2-185.ap-southeast-1.compute.internal</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>i-0c8104214f010bf57</t>
-        </is>
-      </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
-      <c r="N104" t="inlineStr">
-        <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O104" s="2" t="inlineStr">
-        <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53799</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O104"/>
+  <autoFilter ref="A1:O103"/>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O2" r:id="rId1"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O3" r:id="rId2"/>
@@ -10019,7 +9878,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O101" r:id="rId100"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O102" r:id="rId101"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O103" r:id="rId102"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O104" r:id="rId103"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update example outputs and screenshot with First Seen column
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/example-vuln-report.xlsx
+++ b/output/example-vuln-report.xlsx
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'By Package'!$A$1:$H$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'By Host'!$A$1:$I$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Detail'!$A$1:$O$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Detail'!$A$1:$P$103</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -468,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2026-02-18 16:20</t>
+          <t>2026-02-18 16:36</t>
         </is>
       </c>
     </row>
@@ -2225,7 +2225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O103"/>
+  <dimension ref="A1:P103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2243,11 +2243,12 @@
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="49" customWidth="1" min="9" max="9"/>
     <col width="21" customWidth="1" min="10" max="10"/>
-    <col width="16" customWidth="1" min="11" max="11"/>
-    <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="13" customWidth="1" min="13" max="13"/>
-    <col width="16" customWidth="1" min="14" max="14"/>
-    <col width="50" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="19" customWidth="1" min="13" max="13"/>
+    <col width="13" customWidth="1" min="14" max="14"/>
+    <col width="16" customWidth="1" min="15" max="15"/>
+    <col width="50" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2303,25 +2304,30 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>First Seen</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Exploit Public</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Exploit Wormified</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>VM Provider</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Collector Type</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>CVE Link</t>
         </is>
@@ -2376,25 +2382,30 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>2025-07-24</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O2" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
         </is>
@@ -2429,12 +2440,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2.1.4</t>
+          <t>4.0.1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2.5.4</t>
+          <t>4.0.4</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -2449,25 +2460,30 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>2025-07-24</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O3" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
         </is>
@@ -2502,45 +2518,50 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4.0.1</t>
+          <t>2.1.4</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>4.0.4</t>
+          <t>2.5.4</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>2025-07-24</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O4" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P4" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
         </is>
@@ -2585,35 +2606,40 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>2025-07-24</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O5" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-7783</t>
         </is>
@@ -2668,25 +2694,30 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O6" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P6" s="2" t="inlineStr">
         <is>
           <t>https://github.com/advisories/GHSA-vjh7-7g9h-fjfh</t>
         </is>
@@ -2741,25 +2772,30 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O7" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P7" s="2" t="inlineStr">
         <is>
           <t>https://github.com/advisories/GHSA-vjh7-7g9h-fjfh</t>
         </is>
@@ -2814,25 +2850,30 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O8" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P8" s="2" t="inlineStr">
         <is>
           <t>https://github.com/advisories/GHSA-vjh7-7g9h-fjfh</t>
         </is>
@@ -2867,7 +2908,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3.1.2</t>
+          <t>3.0.12</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -2887,25 +2928,30 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O9" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P9" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
         </is>
@@ -2940,7 +2986,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3.0.12</t>
+          <t>3.1.2</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -2960,25 +3006,30 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O10" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P10" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
         </is>
@@ -3033,25 +3084,30 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O11" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P11" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
         </is>
@@ -3106,25 +3162,30 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O12" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P12" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6547</t>
         </is>
@@ -3159,7 +3220,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3.0.17</t>
+          <t>3.0.12</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -3179,25 +3240,30 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O13" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P13" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
         </is>
@@ -3232,7 +3298,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3.0.12</t>
+          <t>3.0.17</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -3252,25 +3318,30 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O14" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P14" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
         </is>
@@ -3325,25 +3396,30 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
+          <t>2025-06-26</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O15" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P15" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
         </is>
@@ -3398,25 +3474,30 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O16" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P16" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-6545</t>
         </is>
@@ -3471,25 +3552,30 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O17" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P17" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-49708</t>
         </is>
@@ -3544,25 +3630,30 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O18" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P18" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2018-3750</t>
         </is>
@@ -3617,25 +3708,30 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O19" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P19" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2022-2421</t>
         </is>
@@ -3690,25 +3786,30 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O20" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P20" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2023-45311</t>
         </is>
@@ -3763,25 +3864,30 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
+      <c r="M21" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O21" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P21" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2023-45311</t>
         </is>
@@ -3836,25 +3942,30 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
+      <c r="M22" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O22" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P22" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10750</t>
         </is>
@@ -3909,25 +4020,30 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
+      <c r="M23" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O23" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P23" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-60724</t>
         </is>
@@ -3982,25 +4098,30 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
+      <c r="M24" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O24" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P24" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
@@ -4055,25 +4176,30 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
+      <c r="M25" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O25" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P25" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
@@ -4128,25 +4254,30 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
+      <c r="M26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O26" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P26" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
@@ -4201,25 +4332,30 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
+      <c r="M27" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O27" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P27" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
@@ -4274,25 +4410,30 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
+      <c r="M28" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O28" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P28" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
@@ -4327,12 +4468,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0.0.8</t>
+          <t>1.2.5</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>0.2.4</t>
+          <t>1.2.6</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -4347,25 +4488,30 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
+      <c r="M29" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O29" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P29" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
@@ -4400,12 +4546,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>1.2.5</t>
+          <t>0.0.8</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1.2.6</t>
+          <t>0.2.4</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -4420,25 +4566,30 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
+      <c r="M30" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O30" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P30" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
@@ -4493,25 +4644,30 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
+      <c r="M31" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O31" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P31" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-44906</t>
         </is>
@@ -4566,25 +4722,30 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
+      <c r="M32" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O32" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P32" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-47981</t>
         </is>
@@ -4639,25 +4800,30 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr">
+      <c r="M33" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O33" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P33" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-59287</t>
         </is>
@@ -4712,25 +4878,30 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr">
+      <c r="M34" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O34" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P34" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53766</t>
         </is>
@@ -4785,25 +4956,30 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr">
+      <c r="M35" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O35" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P35" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-23383</t>
         </is>
@@ -4858,25 +5034,30 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr">
+      <c r="M36" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O36" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P36" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2018-1000620</t>
         </is>
@@ -4931,25 +5112,30 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
+      <c r="M37" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O37" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P37" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-19919</t>
         </is>
@@ -5004,25 +5190,30 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr">
+      <c r="M38" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O38" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P38" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2016-9535</t>
         </is>
@@ -5077,25 +5268,30 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L39" t="inlineStr">
+      <c r="M39" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O39" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P39" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2017-16042</t>
         </is>
@@ -5150,25 +5346,30 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr">
+      <c r="M40" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O40" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P40" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2017-16042</t>
         </is>
@@ -5223,25 +5424,30 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
+      <c r="M41" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O41" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P41" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-3918</t>
         </is>
@@ -5296,25 +5502,30 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr">
+      <c r="M42" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O42" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P42" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-3918</t>
         </is>
@@ -5369,25 +5580,30 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
+      <c r="M43" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O43" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P43" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-23369</t>
         </is>
@@ -5442,25 +5658,30 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
+      <c r="M44" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O44" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P44" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21307</t>
         </is>
@@ -5515,25 +5736,30 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
+      <c r="M45" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O45" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P45" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21298</t>
         </is>
@@ -5588,25 +5814,30 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
+      <c r="M46" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O46" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P46" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2021-31597</t>
         </is>
@@ -5661,25 +5892,30 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
+      <c r="M47" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O47" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P47" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
         </is>
@@ -5734,25 +5970,30 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
+      <c r="M48" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O48" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P48" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
         </is>
@@ -5807,25 +6048,30 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr">
+      <c r="M49" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O49" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P49" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
         </is>
@@ -5880,25 +6126,30 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr">
+      <c r="M50" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O50" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P50" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2019-10744</t>
         </is>
@@ -5953,25 +6204,30 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
+      <c r="M51" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O51" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P51" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2020-36242</t>
         </is>
@@ -6026,25 +6282,30 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
+          <t>2025-08-24</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr">
+      <c r="M52" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O52" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P52" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9288</t>
         </is>
@@ -6099,25 +6360,30 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr">
+      <c r="M53" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O53" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P53" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9288</t>
         </is>
@@ -6172,25 +6438,30 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
+          <t>2025-08-24</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L54" t="inlineStr">
+      <c r="M54" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O54" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P54" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9288</t>
         </is>
@@ -6245,25 +6516,30 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
+          <t>2025-08-24</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L55" t="inlineStr">
+      <c r="M55" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O55" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P55" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
         </is>
@@ -6308,35 +6584,40 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
+          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>i-0799e3a4b56be2630</t>
+          <t>i-0f3c4563f1c12a574</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L56" t="inlineStr">
+      <c r="M56" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O56" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P56" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
         </is>
@@ -6381,35 +6662,40 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>ip-10-100-3-123.ap-southeast-1.compute.internal</t>
+          <t>ip-172-17-2-49.ap-southeast-1.compute.internal</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>i-0f3c4563f1c12a574</t>
+          <t>i-0799e3a4b56be2630</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr">
+      <c r="M57" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O57" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P57" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2025-9287</t>
         </is>
@@ -6464,25 +6750,30 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L58" t="inlineStr">
+      <c r="M58" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O58" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P58" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29966</t>
         </is>
@@ -6537,25 +6828,30 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L59" t="inlineStr">
+      <c r="M59" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O59" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P59" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2023-45133</t>
         </is>
@@ -6610,25 +6906,30 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L60" t="inlineStr">
+      <c r="M60" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O60" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P60" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-54918</t>
         </is>
@@ -6683,25 +6984,30 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr">
+      <c r="M61" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O61" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P61" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-26645</t>
         </is>
@@ -6756,25 +7062,30 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr">
+      <c r="M62" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O62" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P62" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53778</t>
         </is>
@@ -6829,25 +7140,30 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr">
+      <c r="M63" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O63" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P63" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29967</t>
         </is>
@@ -6902,25 +7218,30 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L64" t="inlineStr">
+      <c r="M64" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O64" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P64" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-48822</t>
         </is>
@@ -6975,25 +7296,30 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L65" t="inlineStr">
+      <c r="M65" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O65" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P65" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24084</t>
         </is>
@@ -7048,25 +7374,30 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L66" t="inlineStr">
+      <c r="M66" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O66" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P66" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21295</t>
         </is>
@@ -7121,25 +7452,30 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L67" t="inlineStr">
+      <c r="M67" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O67" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P67" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-26663</t>
         </is>
@@ -7194,25 +7530,30 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr">
+      <c r="M68" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O68" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P68" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24035</t>
         </is>
@@ -7267,25 +7608,30 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L69" t="inlineStr">
+      <c r="M69" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O69" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P69" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21309</t>
         </is>
@@ -7340,25 +7686,30 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L70" t="inlineStr">
+      <c r="M70" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O70" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P70" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-32710</t>
         </is>
@@ -7413,25 +7764,30 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr">
+      <c r="M71" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O71" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P71" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27480</t>
         </is>
@@ -7486,25 +7842,30 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L72" t="inlineStr">
+      <c r="M72" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O72" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P72" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21294</t>
         </is>
@@ -7559,25 +7920,30 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L73" t="inlineStr">
+      <c r="M73" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O73" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P73" s="2" t="inlineStr">
         <is>
           <t>https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2020-28502</t>
         </is>
@@ -7632,25 +7998,30 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L74" t="inlineStr">
+      <c r="M74" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O74" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P74" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21376</t>
         </is>
@@ -7705,25 +8076,30 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L75" t="inlineStr">
+      <c r="M75" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O75" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P75" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-49735</t>
         </is>
@@ -7778,25 +8154,30 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L76" t="inlineStr">
+      <c r="M76" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O76" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P76" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-50177</t>
         </is>
@@ -7851,25 +8232,30 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L77" t="inlineStr">
+      <c r="M77" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O77" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P77" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29828</t>
         </is>
@@ -7924,25 +8310,30 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L78" t="inlineStr">
+      <c r="M78" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O78" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P78" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-33071</t>
         </is>
@@ -7997,25 +8388,30 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L79" t="inlineStr">
+      <c r="M79" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O79" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P79" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21297</t>
         </is>
@@ -8070,25 +8466,30 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L80" t="inlineStr">
+      <c r="M80" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O80" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P80" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-33070</t>
         </is>
@@ -8143,25 +8544,30 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L81" t="inlineStr">
+      <c r="M81" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O81" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P81" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-26670</t>
         </is>
@@ -8216,25 +8622,30 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L82" t="inlineStr">
+      <c r="M82" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O82" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P82" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24045</t>
         </is>
@@ -8289,25 +8700,30 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L83" t="inlineStr">
+      <c r="M83" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O83" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P83" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27482</t>
         </is>
@@ -8362,25 +8778,30 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr">
+      <c r="M84" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O84" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P84" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-24064</t>
         </is>
@@ -8435,25 +8856,30 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr">
+      <c r="M85" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O85" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P85" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55228</t>
         </is>
@@ -8508,25 +8934,30 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr">
+      <c r="M86" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O86" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P86" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-50176</t>
         </is>
@@ -8581,25 +9012,30 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L87" t="inlineStr">
+      <c r="M87" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O87" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P87" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53800</t>
         </is>
@@ -8654,25 +9090,30 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L88" t="inlineStr">
+      <c r="M88" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O88" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P88" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2026-20822</t>
         </is>
@@ -8727,25 +9168,30 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L89" t="inlineStr">
+      <c r="M89" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O89" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P89" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55224</t>
         </is>
@@ -8800,25 +9246,30 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L90" t="inlineStr">
+      <c r="M90" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O90" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P90" s="2" t="inlineStr">
         <is>
           <t>https://github.com/advisories/GHSA-xv2f-5jw4-v95m</t>
         </is>
@@ -8873,25 +9324,30 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L91" t="inlineStr">
+      <c r="M91" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O91" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P91" s="2" t="inlineStr">
         <is>
           <t>https://github.com/advisories/GHSA-xv2f-5jw4-v95m</t>
         </is>
@@ -8946,25 +9402,30 @@
       </c>
       <c r="K92" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L92" t="inlineStr">
+      <c r="M92" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O92" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P92" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-29833</t>
         </is>
@@ -9019,25 +9480,30 @@
       </c>
       <c r="K93" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L93" t="inlineStr">
+      <c r="M93" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O93" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P93" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-26686</t>
         </is>
@@ -9092,25 +9558,30 @@
       </c>
       <c r="K94" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L94" t="inlineStr">
+      <c r="M94" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O94" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P94" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-21296</t>
         </is>
@@ -9165,25 +9636,30 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L95" t="inlineStr">
+      <c r="M95" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O95" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P95" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55236</t>
         </is>
@@ -9238,25 +9714,30 @@
       </c>
       <c r="K96" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L96" t="inlineStr">
+      <c r="M96" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O96" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P96" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-27491</t>
         </is>
@@ -9311,25 +9792,30 @@
       </c>
       <c r="K97" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L97" t="inlineStr">
+      <c r="M97" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O97" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P97" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-60716</t>
         </is>
@@ -9384,25 +9870,30 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L98" t="inlineStr">
+      <c r="M98" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O98" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P98" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-48807</t>
         </is>
@@ -9457,25 +9948,30 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L99" t="inlineStr">
+      <c r="M99" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O99" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P99" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-55226</t>
         </is>
@@ -9530,25 +10026,30 @@
       </c>
       <c r="K100" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L100" t="inlineStr">
+      <c r="M100" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O100" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P100" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-47980</t>
         </is>
@@ -9603,25 +10104,30 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L101" t="inlineStr">
+      <c r="M101" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O101" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P101" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2024-36357</t>
         </is>
@@ -9676,25 +10182,30 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L102" t="inlineStr">
+      <c r="M102" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N102" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O102" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P102" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2024-36350</t>
         </is>
@@ -9749,135 +10260,140 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L103" t="inlineStr">
+      <c r="M103" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>AWS</t>
-        </is>
-      </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>Agentless</t>
-        </is>
-      </c>
-      <c r="O103" s="2" t="inlineStr">
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>Agentless</t>
+        </is>
+      </c>
+      <c r="P103" s="2" t="inlineStr">
         <is>
           <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2025-53799</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O103"/>
+  <autoFilter ref="A1:P103"/>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O9" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O10" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O11" r:id="rId10"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O12" r:id="rId11"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O13" r:id="rId12"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O14" r:id="rId13"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O15" r:id="rId14"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O16" r:id="rId15"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O17" r:id="rId16"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O18" r:id="rId17"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O19" r:id="rId18"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O20" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O21" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O22" r:id="rId21"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O23" r:id="rId22"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O24" r:id="rId23"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O25" r:id="rId24"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O26" r:id="rId25"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O27" r:id="rId26"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O28" r:id="rId27"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O29" r:id="rId28"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O30" r:id="rId29"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O31" r:id="rId30"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O32" r:id="rId31"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O33" r:id="rId32"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O34" r:id="rId33"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O35" r:id="rId34"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O36" r:id="rId35"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O37" r:id="rId36"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O38" r:id="rId37"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O39" r:id="rId38"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O40" r:id="rId39"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O41" r:id="rId40"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O42" r:id="rId41"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O43" r:id="rId42"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O44" r:id="rId43"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O45" r:id="rId44"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O46" r:id="rId45"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O47" r:id="rId46"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O48" r:id="rId47"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O49" r:id="rId48"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O50" r:id="rId49"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O51" r:id="rId50"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O52" r:id="rId51"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O53" r:id="rId52"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O54" r:id="rId53"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O55" r:id="rId54"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O56" r:id="rId55"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O57" r:id="rId56"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O58" r:id="rId57"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O59" r:id="rId58"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O60" r:id="rId59"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O61" r:id="rId60"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O62" r:id="rId61"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O63" r:id="rId62"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O64" r:id="rId63"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O65" r:id="rId64"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O66" r:id="rId65"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O67" r:id="rId66"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O68" r:id="rId67"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O69" r:id="rId68"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O70" r:id="rId69"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O71" r:id="rId70"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O72" r:id="rId71"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O73" r:id="rId72"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O74" r:id="rId73"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O75" r:id="rId74"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O76" r:id="rId75"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O77" r:id="rId76"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O78" r:id="rId77"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O79" r:id="rId78"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O80" r:id="rId79"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O81" r:id="rId80"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O82" r:id="rId81"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O83" r:id="rId82"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O84" r:id="rId83"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O85" r:id="rId84"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O86" r:id="rId85"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O87" r:id="rId86"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O88" r:id="rId87"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O89" r:id="rId88"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O90" r:id="rId89"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O91" r:id="rId90"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O92" r:id="rId91"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O93" r:id="rId92"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O94" r:id="rId93"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O95" r:id="rId94"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O96" r:id="rId95"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O97" r:id="rId96"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O98" r:id="rId97"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O99" r:id="rId98"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O100" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O101" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O102" r:id="rId101"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O103" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P12" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P13" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P14" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P15" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P16" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P17" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P18" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P19" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P20" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P21" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P22" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P23" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P24" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P25" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P26" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P27" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P28" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P29" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P30" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P31" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P32" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P33" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P34" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P35" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P36" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P37" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P39" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P40" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P41" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P42" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P43" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P44" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P45" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P46" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P47" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P48" r:id="rId47"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P49" r:id="rId48"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P50" r:id="rId49"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P51" r:id="rId50"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P52" r:id="rId51"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P53" r:id="rId52"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P54" r:id="rId53"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P55" r:id="rId54"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P56" r:id="rId55"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P57" r:id="rId56"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P58" r:id="rId57"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P59" r:id="rId58"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P60" r:id="rId59"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P61" r:id="rId60"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P62" r:id="rId61"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P63" r:id="rId62"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P64" r:id="rId63"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P65" r:id="rId64"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P66" r:id="rId65"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P67" r:id="rId66"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P68" r:id="rId67"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P69" r:id="rId68"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P70" r:id="rId69"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P71" r:id="rId70"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P72" r:id="rId71"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P73" r:id="rId72"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P74" r:id="rId73"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P75" r:id="rId74"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P76" r:id="rId75"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P77" r:id="rId76"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P78" r:id="rId77"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P79" r:id="rId78"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P80" r:id="rId79"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P81" r:id="rId80"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P82" r:id="rId81"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P83" r:id="rId82"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P84" r:id="rId83"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P85" r:id="rId84"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P86" r:id="rId85"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P87" r:id="rId86"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P88" r:id="rId87"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P89" r:id="rId88"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P90" r:id="rId89"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P91" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P92" r:id="rId91"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P93" r:id="rId92"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P94" r:id="rId93"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P95" r:id="rId94"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P96" r:id="rId95"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P97" r:id="rId96"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P98" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P99" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P100" r:id="rId99"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P101" r:id="rId100"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P102" r:id="rId101"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="P103" r:id="rId102"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>